<commit_message>
Created File Modified "Fixed A Copy Issue"
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/CDD/Internal-Audit.xlsx
+++ b/Software Specification/Architecture/CDD/Internal-Audit.xlsx
@@ -3,22 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74525084-EB5F-4E73-8465-9DD43351808A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC30BF2-C2EC-4C77-BD74-9518B2CDA1BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GDD review" sheetId="5" r:id="rId1"/>
-    <sheet name="LED CDD" sheetId="6" r:id="rId2"/>
-    <sheet name="DIO CDD" sheetId="7" r:id="rId3"/>
-    <sheet name="External_ISR CDD" sheetId="8" r:id="rId4"/>
+    <sheet name="LED CDD" sheetId="6" r:id="rId1"/>
+    <sheet name="DIO CDD" sheetId="7" r:id="rId2"/>
+    <sheet name="External_ISR CDD" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>Review point</t>
   </si>
@@ -27,9 +26,6 @@
   </si>
   <si>
     <t>Reviewer</t>
-  </si>
-  <si>
-    <t>Ali</t>
   </si>
   <si>
     <t>Point status</t>
@@ -41,57 +37,7 @@
     <t>Acceptance</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>Version</t>
-  </si>
-  <si>
-    <t>Remove Delay &amp; Std_Types from application CDD</t>
-  </si>
-  <si>
-    <t>Req_ID for all requirements is wrong it's a CDD document it should have it's own Req_ID which covers a GDD requirement</t>
-  </si>
-  <si>
-    <t>13/3/2020</t>
-  </si>
-  <si>
-    <t>VoidLED_Animation_RunModeOne(void):
-Descripe mode 1 algorithm in the flow graph</t>
-  </si>
-  <si>
-    <t>VoidLED_Animation_RunModeTwo(void):
-Descripe mode 1 algorithm in the flow graph</t>
-  </si>
-  <si>
-    <t>VoidLED_Animation_RunTi_Right(void):
-Descripe Right TI animation algorithm in the flow graph</t>
-  </si>
-  <si>
-    <t>VoidLED_Animation_RunTI_Left(void):
-Descripe Left TI animation algorithm in the flow graph</t>
-  </si>
-  <si>
-    <t>Pin checking shall be done here to decide the error status</t>
-  </si>
-  <si>
-    <t>ERROR_T LED_SetLedON(uint8_t ledNumber):
-Flow graph shall descripe how LED will be on (by calling which function?)
-And how you will know LED is ON/OFF ! You will read the output ?</t>
-  </si>
-  <si>
-    <t>ERROR_t LED_SetLedOFF(uint8_t ledNumber):
-Same as the prev. point</t>
-  </si>
-  <si>
-    <t>DIO flow graphs shall be in the same table of the fuctions</t>
-  </si>
-  <si>
-    <t>ERROR_t LED_Animation_Init(void):
-The pin number checking will be done in Switch/LED init not inside this function so remove the checking from the flow graph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In DIO_GetPinvalue function it's not "show output as high/low" it should be "Set the uint8_t* value with LOW/HIGH" </t>
   </si>
 </sst>
 </file>
@@ -172,50 +118,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <font>
         <condense val="0"/>
@@ -764,212 +667,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="F2:F8">
-    <cfRule type="containsText" dxfId="29" priority="128" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="129" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="130" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E8">
-    <cfRule type="cellIs" dxfId="26" priority="123" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="124" operator="equal">
-      <formula>"Accepted"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"Accepted, Rejected"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>"Open, Closed"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,92 +693,52 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
@@ -1118,12 +780,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,56 +806,36 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="A2" s="5"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1278,12 +920,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,19 +947,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
External Interrurpt, Application, And Document Structure Reviewed
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/CDD/Internal-Audit.xlsx
+++ b/Software Specification/Architecture/CDD/Internal-Audit.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC30BF2-C2EC-4C77-BD74-9518B2CDA1BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BC2983-ADF6-4D84-87E7-9974F0AFBD13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LED CDD" sheetId="6" r:id="rId1"/>
     <sheet name="DIO CDD" sheetId="7" r:id="rId2"/>
     <sheet name="External_ISR CDD" sheetId="8" r:id="rId3"/>
+    <sheet name="Document Structure" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
   <si>
     <t>Review point</t>
   </si>
@@ -38,6 +39,24 @@
   </si>
   <si>
     <t>Version</t>
+  </si>
+  <si>
+    <t>13/03/2020</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Flow Charts are drawn outside the APIs tables</t>
+  </si>
+  <si>
+    <t>DIO Flow Charts are drawn between the External_ISR APIs and their Flow Charts</t>
+  </si>
+  <si>
+    <t>Content Table is not updated</t>
+  </si>
+  <si>
+    <t>You can update it automatically using microsoft word</t>
   </si>
 </sst>
 </file>
@@ -88,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -114,11 +133,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -670,7 +781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -750,21 +861,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F6">
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="34" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="4" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="32" priority="5" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -871,40 +982,40 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F7">
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="29" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="27" priority="10" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F7">
-    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -922,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,49 +1074,71 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="6"/>
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
     </row>
+    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="F2">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1019,4 +1152,116 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621809EB-4494-4308-9D51-080EDDA92631}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="48.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{CE61DC3D-9F8A-40B0-B5E0-C5D3720A59A3}">
+      <formula1>"Accepted, Rejected"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{7BCA0151-2CD4-4D66-87C6-0DC2B4DC5D5F}">
+      <formula1>"Open, Closed"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>